<commit_message>
Final project update - README, License, Agile Docs, UI Improvements
</commit_message>
<xml_diff>
--- a/docs/Unit_Test_Plan_v0.1.xlsx
+++ b/docs/Unit_Test_Plan_v0.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d79fe2bc3d7eff9/Desktop/AI-Enabled-Recommendation-Engine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d79fe2bc3d7eff9/Desktop/AI_Ecommerce_project/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{3B9D4FEA-5A3F-460B-9A40-165575443B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{570631C3-5C73-439B-9A83-188487BE26CD}"/>
+  <xr:revisionPtr revIDLastSave="438" documentId="8_{3B9D4FEA-5A3F-460B-9A40-165575443B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADB3854D-0F3B-4FC7-84D9-FC6B59313BC5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C3B83BB6-2AB9-4547-8541-9F6969E92BF1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>Actual Result</t>
   </si>
@@ -54,19 +54,223 @@
     <t>Sl: No:</t>
   </si>
   <si>
-    <t>Precision Calculation Test</t>
-  </si>
-  <si>
-    <t>Run model3_evalution.py with sample actual and recommended item</t>
-  </si>
-  <si>
-    <t>Precision is calculated correctly.</t>
-  </si>
-  <si>
-    <t>Precision value should be between 0 and 1.</t>
-  </si>
-  <si>
-    <t>Precision calcalated successfully</t>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>User Registration- Valid input</t>
+  </si>
+  <si>
+    <t>Enter valid name, email, password click Register</t>
+  </si>
+  <si>
+    <t>All fields contain valid data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User account created successfully </t>
+  </si>
+  <si>
+    <t>User Registration-Duplicate Email</t>
+  </si>
+  <si>
+    <t>Enter already registered email and submit</t>
+  </si>
+  <si>
+    <t>Email already exists in database</t>
+  </si>
+  <si>
+    <t>Error message "Email already registered"</t>
+  </si>
+  <si>
+    <t>User Login-Valid Credentials</t>
+  </si>
+  <si>
+    <t>Enter cōrrect email and password</t>
+  </si>
+  <si>
+    <t>Redirect to home/dashboard page</t>
+  </si>
+  <si>
+    <t>Valid login credentials</t>
+  </si>
+  <si>
+    <t>User Login-invalid Password</t>
+  </si>
+  <si>
+    <t>Enter correct email but wrong password</t>
+  </si>
+  <si>
+    <t>Invalid password</t>
+  </si>
+  <si>
+    <t>Error message displayed</t>
+  </si>
+  <si>
+    <t>Logout Functionality</t>
+  </si>
+  <si>
+    <t>Click logout button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User session active </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User redicted to login page </t>
+  </si>
+  <si>
+    <t>Products avaliable in database</t>
+  </si>
+  <si>
+    <t>Product Listing Display</t>
+  </si>
+  <si>
+    <t>Open homepage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asll product displayed properly </t>
+  </si>
+  <si>
+    <t>Product image Load</t>
+  </si>
+  <si>
+    <t>check product images on homepage</t>
+  </si>
+  <si>
+    <t>Valid image path in database</t>
+  </si>
+  <si>
+    <t>image load without error</t>
+  </si>
+  <si>
+    <t>Add  Product to Cart</t>
+  </si>
+  <si>
+    <t>Click "Add to Cart"</t>
+  </si>
+  <si>
+    <t>Product added successfully</t>
+  </si>
+  <si>
+    <t>Product available</t>
+  </si>
+  <si>
+    <t>Remove Product from Cart</t>
+  </si>
+  <si>
+    <t>Product exists in cart</t>
+  </si>
+  <si>
+    <t>Product removed successfully</t>
+  </si>
+  <si>
+    <t>Click "remove button"</t>
+  </si>
+  <si>
+    <t>Cart Tatal Calcuation</t>
+  </si>
+  <si>
+    <t>Add multiple products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple product in cart </t>
+  </si>
+  <si>
+    <t>Correct total amount displayed</t>
+  </si>
+  <si>
+    <t>Proceed to checkout</t>
+  </si>
+  <si>
+    <t>Click checkout button</t>
+  </si>
+  <si>
+    <t>Cart not empty</t>
+  </si>
+  <si>
+    <t>Redirect to payment gateway</t>
+  </si>
+  <si>
+    <t>Successful Payment</t>
+  </si>
+  <si>
+    <t>Complete payment using Razorpay</t>
+  </si>
+  <si>
+    <t>Valid payment</t>
+  </si>
+  <si>
+    <t>Order saved in database</t>
+  </si>
+  <si>
+    <t>Failed Payment Handling</t>
+  </si>
+  <si>
+    <t>Cancel payment</t>
+  </si>
+  <si>
+    <t>Payment failure</t>
+  </si>
+  <si>
+    <t>order not created</t>
+  </si>
+  <si>
+    <t>Order Histroy Display</t>
+  </si>
+  <si>
+    <t>order exist</t>
+  </si>
+  <si>
+    <t>Orders displayed correctly</t>
+  </si>
+  <si>
+    <t>Open order history page</t>
+  </si>
+  <si>
+    <t>Invoice Generation</t>
+  </si>
+  <si>
+    <t>Click "download invoice"</t>
+  </si>
+  <si>
+    <t>order completed</t>
+  </si>
+  <si>
+    <t>PDF ibvoice generated</t>
+  </si>
+  <si>
+    <t>AI Recommendation Display</t>
+  </si>
+  <si>
+    <t>Open product details page</t>
+  </si>
+  <si>
+    <t>Similar category products exist</t>
+  </si>
+  <si>
+    <t>Recommended products shown</t>
+  </si>
+  <si>
+    <t>AI Recommendation Accuracy</t>
+  </si>
+  <si>
+    <t>View different categories</t>
+  </si>
+  <si>
+    <t>Matching category logic</t>
+  </si>
+  <si>
+    <t>Relevant recommendations displayed</t>
+  </si>
+  <si>
+    <t>Unauthorized Access Restriction</t>
+  </si>
+  <si>
+    <t>Try accessing dashboard without login</t>
+  </si>
+  <si>
+    <t>User not auhenticated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirect to login page </t>
   </si>
 </sst>
 </file>
@@ -80,26 +284,25 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="14"/>
+      <color indexed="56"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF003366"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="56"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -118,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -127,40 +330,141 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -178,6 +482,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -477,96 +785,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF95B16C-182C-4757-B929-A728708A2DB0}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.08984375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="26.26953125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="31.26953125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="32.6328125" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="8.1796875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="39.54296875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="36.6328125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="34.7265625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="13" customFormat="1" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+    <row r="2" spans="1:7" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>